<commit_message>
focus on riders informations
</commit_message>
<xml_diff>
--- a/race.xlsx
+++ b/race.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucafr-my.sharepoint.com/personal/viny_presty_nakavoua_nsaloumouna_etu_uca_fr/Documents/2A/collecte_auto_donnees/S4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_7B1172ABD3B05A211B1A3C11595ED87656CD2120" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{233C8B2B-CC83-4E16-8DB6-366CD3300377}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_7B1172ABD3B05A211B1A3C11595ED87656CD2120" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FA2853A-BE52-43F8-A4F6-614698C67C75}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -779,6 +779,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1072,6 +1076,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>

</xml_diff>